<commit_message>
Added Federal Compensation statistic for the output data table
</commit_message>
<xml_diff>
--- a/Michigan Dataset.xlsx
+++ b/Michigan Dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Number of HUBZone Businesses</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -454,6 +459,9 @@
       <c r="B2" t="n">
         <v>9</v>
       </c>
+      <c r="C2" t="n">
+        <v>147820.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -464,6 +472,9 @@
       <c r="B3" t="n">
         <v>4</v>
       </c>
+      <c r="C3" t="n">
+        <v>215157.64</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -474,6 +485,9 @@
       <c r="B4" t="n">
         <v>0</v>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -484,6 +498,9 @@
       <c r="B5" t="n">
         <v>7</v>
       </c>
+      <c r="C5" t="n">
+        <v>1370792.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -494,6 +511,9 @@
       <c r="B6" t="n">
         <v>23</v>
       </c>
+      <c r="C6" t="n">
+        <v>61639375.49</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -504,6 +524,9 @@
       <c r="B7" t="n">
         <v>7</v>
       </c>
+      <c r="C7" t="n">
+        <v>6483870.44</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -514,6 +537,9 @@
       <c r="B8" t="n">
         <v>8</v>
       </c>
+      <c r="C8" t="n">
+        <v>3231566.22</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -524,6 +550,9 @@
       <c r="B9" t="n">
         <v>0</v>
       </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -534,6 +563,9 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -544,6 +576,9 @@
       <c r="B11" t="n">
         <v>13</v>
       </c>
+      <c r="C11" t="n">
+        <v>86482253.62</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -554,6 +589,9 @@
       <c r="B12" t="n">
         <v>2</v>
       </c>
+      <c r="C12" t="n">
+        <v>380477</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -564,6 +602,9 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -574,6 +615,9 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -584,6 +628,9 @@
       <c r="B15" t="n">
         <v>0</v>
       </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -594,6 +641,9 @@
       <c r="B16" t="n">
         <v>1</v>
       </c>
+      <c r="C16" t="n">
+        <v>3600.99</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -604,6 +654,9 @@
       <c r="B17" t="n">
         <v>32</v>
       </c>
+      <c r="C17" t="n">
+        <v>111280345.73</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -614,6 +667,9 @@
       <c r="B18" t="n">
         <v>1</v>
       </c>
+      <c r="C18" t="n">
+        <v>79663</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -624,6 +680,9 @@
       <c r="B19" t="n">
         <v>12</v>
       </c>
+      <c r="C19" t="n">
+        <v>408668.69</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -634,6 +693,9 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -644,6 +706,9 @@
       <c r="B21" t="n">
         <v>23</v>
       </c>
+      <c r="C21" t="n">
+        <v>8155410.51</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -654,6 +719,9 @@
       <c r="B22" t="n">
         <v>21</v>
       </c>
+      <c r="C22" t="n">
+        <v>96224475.73999999</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -664,6 +732,9 @@
       <c r="B23" t="n">
         <v>8</v>
       </c>
+      <c r="C23" t="n">
+        <v>12075683.78</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -674,6 +745,9 @@
       <c r="B24" t="n">
         <v>0</v>
       </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -684,6 +758,9 @@
       <c r="B25" t="n">
         <v>13</v>
       </c>
+      <c r="C25" t="n">
+        <v>349409.25</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -694,6 +771,9 @@
       <c r="B26" t="n">
         <v>35</v>
       </c>
+      <c r="C26" t="n">
+        <v>7607370.51</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -704,6 +784,9 @@
       <c r="B27" t="n">
         <v>7</v>
       </c>
+      <c r="C27" t="n">
+        <v>568311.13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -714,6 +797,9 @@
       <c r="B28" t="n">
         <v>17</v>
       </c>
+      <c r="C28" t="n">
+        <v>4226963.22</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -724,6 +810,9 @@
       <c r="B29" t="n">
         <v>10</v>
       </c>
+      <c r="C29" t="n">
+        <v>228754.85</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -734,6 +823,9 @@
       <c r="B30" t="n">
         <v>9</v>
       </c>
+      <c r="C30" t="n">
+        <v>7641129.11</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -744,6 +836,9 @@
       <c r="B31" t="n">
         <v>1</v>
       </c>
+      <c r="C31" t="n">
+        <v>38600.28</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -754,6 +849,9 @@
       <c r="B32" t="n">
         <v>67</v>
       </c>
+      <c r="C32" t="n">
+        <v>42547594.5</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -764,6 +862,9 @@
       <c r="B33" t="n">
         <v>3</v>
       </c>
+      <c r="C33" t="n">
+        <v>65141.88</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -774,6 +875,9 @@
       <c r="B34" t="n">
         <v>1</v>
       </c>
+      <c r="C34" t="n">
+        <v>1417.4</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -784,6 +888,9 @@
       <c r="B35" t="n">
         <v>0</v>
       </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -794,6 +901,9 @@
       <c r="B36" t="n">
         <v>28</v>
       </c>
+      <c r="C36" t="n">
+        <v>12825763.36</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -804,6 +914,9 @@
       <c r="B37" t="n">
         <v>6</v>
       </c>
+      <c r="C37" t="n">
+        <v>650467.25</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -814,6 +927,9 @@
       <c r="B38" t="n">
         <v>1</v>
       </c>
+      <c r="C38" t="n">
+        <v>55100</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -824,6 +940,9 @@
       <c r="B39" t="n">
         <v>1</v>
       </c>
+      <c r="C39" t="n">
+        <v>514166.44</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -834,6 +953,9 @@
       <c r="B40" t="n">
         <v>16</v>
       </c>
+      <c r="C40" t="n">
+        <v>53758188.34</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -844,6 +966,9 @@
       <c r="B41" t="n">
         <v>0</v>
       </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -854,6 +979,9 @@
       <c r="B42" t="n">
         <v>22</v>
       </c>
+      <c r="C42" t="n">
+        <v>33374734.17</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -864,6 +992,9 @@
       <c r="B43" t="n">
         <v>0</v>
       </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -874,6 +1005,9 @@
       <c r="B44" t="n">
         <v>0</v>
       </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -884,6 +1018,9 @@
       <c r="B45" t="n">
         <v>1</v>
       </c>
+      <c r="C45" t="n">
+        <v>240655</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -894,6 +1031,9 @@
       <c r="B46" t="n">
         <v>0</v>
       </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -904,6 +1044,9 @@
       <c r="B47" t="n">
         <v>2</v>
       </c>
+      <c r="C47" t="n">
+        <v>1216175.75</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -914,6 +1057,9 @@
       <c r="B48" t="n">
         <v>0</v>
       </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -924,6 +1070,9 @@
       <c r="B49" t="n">
         <v>36</v>
       </c>
+      <c r="C49" t="n">
+        <v>78487432.45</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -934,6 +1083,9 @@
       <c r="B50" t="n">
         <v>0</v>
       </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -944,6 +1096,9 @@
       <c r="B51" t="n">
         <v>4</v>
       </c>
+      <c r="C51" t="n">
+        <v>1823625.13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -954,6 +1109,9 @@
       <c r="B52" t="n">
         <v>6</v>
       </c>
+      <c r="C52" t="n">
+        <v>89726.92999999999</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -964,6 +1122,9 @@
       <c r="B53" t="n">
         <v>14</v>
       </c>
+      <c r="C53" t="n">
+        <v>5243408.53</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -974,6 +1135,9 @@
       <c r="B54" t="n">
         <v>8</v>
       </c>
+      <c r="C54" t="n">
+        <v>4511160.52</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -984,6 +1148,9 @@
       <c r="B55" t="n">
         <v>0</v>
       </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -994,6 +1161,9 @@
       <c r="B56" t="n">
         <v>6</v>
       </c>
+      <c r="C56" t="n">
+        <v>7224392.34</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -1004,6 +1174,9 @@
       <c r="B57" t="n">
         <v>0</v>
       </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1014,6 +1187,9 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1024,6 +1200,9 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -1034,6 +1213,9 @@
       <c r="B60" t="n">
         <v>21</v>
       </c>
+      <c r="C60" t="n">
+        <v>17276567.55</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -1044,6 +1226,9 @@
       <c r="B61" t="n">
         <v>2</v>
       </c>
+      <c r="C61" t="n">
+        <v>309009.69</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -1054,6 +1239,9 @@
       <c r="B62" t="n">
         <v>8</v>
       </c>
+      <c r="C62" t="n">
+        <v>55776518.4</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -1064,6 +1252,9 @@
       <c r="B63" t="n">
         <v>0</v>
       </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -1074,6 +1265,9 @@
       <c r="B64" t="n">
         <v>52</v>
       </c>
+      <c r="C64" t="n">
+        <v>58185439.92</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -1084,6 +1278,9 @@
       <c r="B65" t="n">
         <v>3</v>
       </c>
+      <c r="C65" t="n">
+        <v>8165960.16</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -1094,6 +1291,9 @@
       <c r="B66" t="n">
         <v>3</v>
       </c>
+      <c r="C66" t="n">
+        <v>108452.7</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -1104,6 +1304,9 @@
       <c r="B67" t="n">
         <v>2</v>
       </c>
+      <c r="C67" t="n">
+        <v>8200</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -1114,6 +1317,9 @@
       <c r="B68" t="n">
         <v>19</v>
       </c>
+      <c r="C68" t="n">
+        <v>12264562.82</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -1124,6 +1330,9 @@
       <c r="B69" t="n">
         <v>1</v>
       </c>
+      <c r="C69" t="n">
+        <v>45064.24</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -1134,6 +1343,9 @@
       <c r="B70" t="n">
         <v>2</v>
       </c>
+      <c r="C70" t="n">
+        <v>347395.52</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -1144,6 +1356,9 @@
       <c r="B71" t="n">
         <v>7</v>
       </c>
+      <c r="C71" t="n">
+        <v>6975560.97</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -1154,6 +1369,9 @@
       <c r="B72" t="n">
         <v>5</v>
       </c>
+      <c r="C72" t="n">
+        <v>865034.62</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -1164,6 +1382,9 @@
       <c r="B73" t="n">
         <v>0</v>
       </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -1174,6 +1395,9 @@
       <c r="B74" t="n">
         <v>1</v>
       </c>
+      <c r="C74" t="n">
+        <v>11686</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -1184,6 +1408,9 @@
       <c r="B75" t="n">
         <v>11</v>
       </c>
+      <c r="C75" t="n">
+        <v>1424479.58</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -1194,6 +1421,9 @@
       <c r="B76" t="n">
         <v>2</v>
       </c>
+      <c r="C76" t="n">
+        <v>357106</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -1204,6 +1434,9 @@
       <c r="B77" t="n">
         <v>5</v>
       </c>
+      <c r="C77" t="n">
+        <v>192024.89</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -1214,6 +1447,9 @@
       <c r="B78" t="n">
         <v>0</v>
       </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -1224,6 +1460,9 @@
       <c r="B79" t="n">
         <v>4</v>
       </c>
+      <c r="C79" t="n">
+        <v>70737.34</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -1234,6 +1473,9 @@
       <c r="B80" t="n">
         <v>6</v>
       </c>
+      <c r="C80" t="n">
+        <v>12619245.46</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -1244,6 +1486,9 @@
       <c r="B81" t="n">
         <v>0</v>
       </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -1254,6 +1499,9 @@
       <c r="B82" t="n">
         <v>18</v>
       </c>
+      <c r="C82" t="n">
+        <v>6525493.61</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -1264,6 +1512,9 @@
       <c r="B83" t="n">
         <v>141</v>
       </c>
+      <c r="C83" t="n">
+        <v>208230619.67</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -1273,6 +1524,9 @@
       </c>
       <c r="B84" t="n">
         <v>29</v>
+      </c>
+      <c r="C84" t="n">
+        <v>5772160.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated Federal Contract Compensation by Year
</commit_message>
<xml_diff>
--- a/Michigan Dataset.xlsx
+++ b/Michigan Dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,77 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Federal Contract Compensation</t>
+          <t>Federal Contract Compensation - 2008</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2009</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2010</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2011</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2012</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2013</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2014</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2015</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2016</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2017</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2018</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2019</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2020</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2021</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Federal Contract Compensation - 2022</t>
         </is>
       </c>
     </row>
@@ -460,7 +530,49 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>147820.5</v>
+        <v>1712.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>107058</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>12600</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3750</v>
+      </c>
+      <c r="J2" t="n">
+        <v>13200</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +585,49 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>215157.64</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>44633.14</v>
+      </c>
+      <c r="K3" t="n">
+        <v>62214.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>9960</v>
+      </c>
+      <c r="M3" t="n">
+        <v>98350</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -488,6 +642,48 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -499,7 +695,49 @@
         <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>1370792.5</v>
+        <v>831586</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>512700.5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8483</v>
+      </c>
+      <c r="H5" t="n">
+        <v>12485</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5538</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +750,49 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>61639375.49</v>
+        <v>4847056.34</v>
+      </c>
+      <c r="D6" t="n">
+        <v>18488102.65</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20318945.55</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12999344.8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>933927.4399999999</v>
+      </c>
+      <c r="H6" t="n">
+        <v>235747</v>
+      </c>
+      <c r="I6" t="n">
+        <v>98790.06</v>
+      </c>
+      <c r="J6" t="n">
+        <v>42024</v>
+      </c>
+      <c r="K6" t="n">
+        <v>173232.4</v>
+      </c>
+      <c r="L6" t="n">
+        <v>378267.54</v>
+      </c>
+      <c r="M6" t="n">
+        <v>66871</v>
+      </c>
+      <c r="N6" t="n">
+        <v>3057066.71</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +805,49 @@
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>6483870.44</v>
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2725</v>
+      </c>
+      <c r="E7" t="n">
+        <v>460136</v>
+      </c>
+      <c r="F7" t="n">
+        <v>108075</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4971254</v>
+      </c>
+      <c r="H7" t="n">
+        <v>104001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>832710</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4969.44</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +860,49 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>3231566.22</v>
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1637350.76</v>
+      </c>
+      <c r="G8" t="n">
+        <v>76410</v>
+      </c>
+      <c r="H8" t="n">
+        <v>36072.62</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>108585.4</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>11420</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1354154.2</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6083.8</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1489.44</v>
       </c>
     </row>
     <row r="9">
@@ -553,6 +917,48 @@
       <c r="C9" t="n">
         <v>0</v>
       </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -566,6 +972,48 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -577,7 +1025,49 @@
         <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>86482253.62</v>
+        <v>5781905</v>
+      </c>
+      <c r="D11" t="n">
+        <v>13802950</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5229554</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1276350</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>8373940</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3445700</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3655950</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2668396.5</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9163795</v>
+      </c>
+      <c r="N11" t="n">
+        <v>10455140</v>
+      </c>
+      <c r="O11" t="n">
+        <v>18308443.12</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4320130</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -590,7 +1080,49 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>380477</v>
+        <v>198748</v>
+      </c>
+      <c r="D12" t="n">
+        <v>181729</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -605,6 +1137,48 @@
       <c r="C13" t="n">
         <v>0</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -618,6 +1192,48 @@
       <c r="C14" t="n">
         <v>0</v>
       </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -631,6 +1247,48 @@
       <c r="C15" t="n">
         <v>0</v>
       </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -642,7 +1300,49 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
         <v>3600.99</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -655,7 +1355,49 @@
         <v>32</v>
       </c>
       <c r="C17" t="n">
-        <v>111280345.73</v>
+        <v>3807976.32</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2555795</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4304547.14</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1623062.16</v>
+      </c>
+      <c r="G17" t="n">
+        <v>716559.03</v>
+      </c>
+      <c r="H17" t="n">
+        <v>260348.16</v>
+      </c>
+      <c r="I17" t="n">
+        <v>12897576.2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>7612218.77</v>
+      </c>
+      <c r="K17" t="n">
+        <v>6083490.52</v>
+      </c>
+      <c r="L17" t="n">
+        <v>7962949.39</v>
+      </c>
+      <c r="M17" t="n">
+        <v>12526074</v>
+      </c>
+      <c r="N17" t="n">
+        <v>19784788.75</v>
+      </c>
+      <c r="O17" t="n">
+        <v>18564322</v>
+      </c>
+      <c r="P17" t="n">
+        <v>12580638.29</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -670,6 +1412,48 @@
       <c r="C18" t="n">
         <v>79663</v>
       </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -681,7 +1465,49 @@
         <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>408668.69</v>
+        <v>204338</v>
+      </c>
+      <c r="D19" t="n">
+        <v>88319.07000000001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>56365.08</v>
+      </c>
+      <c r="F19" t="n">
+        <v>16582</v>
+      </c>
+      <c r="G19" t="n">
+        <v>43064.54</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -696,6 +1522,48 @@
       <c r="C20" t="n">
         <v>0</v>
       </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -707,7 +1575,49 @@
         <v>23</v>
       </c>
       <c r="C21" t="n">
-        <v>8155410.51</v>
+        <v>229332.86</v>
+      </c>
+      <c r="D21" t="n">
+        <v>99937.7</v>
+      </c>
+      <c r="E21" t="n">
+        <v>315886</v>
+      </c>
+      <c r="F21" t="n">
+        <v>262825.2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>368687.37</v>
+      </c>
+      <c r="H21" t="n">
+        <v>170325.93</v>
+      </c>
+      <c r="I21" t="n">
+        <v>480044.3</v>
+      </c>
+      <c r="J21" t="n">
+        <v>610818.0699999999</v>
+      </c>
+      <c r="K21" t="n">
+        <v>823717.7</v>
+      </c>
+      <c r="L21" t="n">
+        <v>729368.48</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1371427.9</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1427425.5</v>
+      </c>
+      <c r="O21" t="n">
+        <v>402605.83</v>
+      </c>
+      <c r="P21" t="n">
+        <v>731412.13</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>131595.54</v>
       </c>
     </row>
     <row r="22">
@@ -720,7 +1630,49 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>96224475.73999999</v>
+        <v>13970874</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16642823.13</v>
+      </c>
+      <c r="E22" t="n">
+        <v>13502641.38</v>
+      </c>
+      <c r="F22" t="n">
+        <v>25241715.65</v>
+      </c>
+      <c r="G22" t="n">
+        <v>23296210.9</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3146459.51</v>
+      </c>
+      <c r="I22" t="n">
+        <v>417984.25</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3970</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1796.92</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -733,7 +1685,49 @@
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>12075683.78</v>
+        <v>1968654.84</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1081822.99</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1537608.65</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3369875.1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>602903.8100000001</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3398737.17</v>
+      </c>
+      <c r="K23" t="n">
+        <v>116081.22</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -748,6 +1742,48 @@
       <c r="C24" t="n">
         <v>0</v>
       </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -759,7 +1795,49 @@
         <v>13</v>
       </c>
       <c r="C25" t="n">
-        <v>349409.25</v>
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>11422.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10567.2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>178743.25</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17852.99</v>
+      </c>
+      <c r="H25" t="n">
+        <v>17342</v>
+      </c>
+      <c r="I25" t="n">
+        <v>14222.75</v>
+      </c>
+      <c r="J25" t="n">
+        <v>4377</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>79229.25</v>
+      </c>
+      <c r="M25" t="n">
+        <v>3576</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>12076.31</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -772,7 +1850,49 @@
         <v>35</v>
       </c>
       <c r="C26" t="n">
-        <v>7607370.51</v>
+        <v>60383.03</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>210404.4</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2501650.53</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1277774.52</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1577481</v>
+      </c>
+      <c r="I26" t="n">
+        <v>106823.91</v>
+      </c>
+      <c r="J26" t="n">
+        <v>51330</v>
+      </c>
+      <c r="K26" t="n">
+        <v>273759.21</v>
+      </c>
+      <c r="L26" t="n">
+        <v>396323.83</v>
+      </c>
+      <c r="M26" t="n">
+        <v>502325.56</v>
+      </c>
+      <c r="N26" t="n">
+        <v>328751.52</v>
+      </c>
+      <c r="O26" t="n">
+        <v>290738</v>
+      </c>
+      <c r="P26" t="n">
+        <v>29625</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -785,7 +1905,49 @@
         <v>7</v>
       </c>
       <c r="C27" t="n">
-        <v>568311.13</v>
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5779.55</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>20700</v>
+      </c>
+      <c r="G27" t="n">
+        <v>446000</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>17147.02</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>13498.92</v>
+      </c>
+      <c r="L27" t="n">
+        <v>65185.64</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -798,7 +1960,49 @@
         <v>17</v>
       </c>
       <c r="C28" t="n">
-        <v>4226963.22</v>
+        <v>197393.91</v>
+      </c>
+      <c r="D28" t="n">
+        <v>27451.75</v>
+      </c>
+      <c r="E28" t="n">
+        <v>24419.28</v>
+      </c>
+      <c r="F28" t="n">
+        <v>754083.98</v>
+      </c>
+      <c r="G28" t="n">
+        <v>98936.50999999999</v>
+      </c>
+      <c r="H28" t="n">
+        <v>992103.87</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>218177.18</v>
+      </c>
+      <c r="K28" t="n">
+        <v>33420</v>
+      </c>
+      <c r="L28" t="n">
+        <v>991520.84</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>889455.9</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -811,7 +2015,49 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>228754.85</v>
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>57984</v>
+      </c>
+      <c r="F29" t="n">
+        <v>52748.89</v>
+      </c>
+      <c r="G29" t="n">
+        <v>98837.96000000001</v>
+      </c>
+      <c r="H29" t="n">
+        <v>19184</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -824,7 +2070,49 @@
         <v>9</v>
       </c>
       <c r="C30" t="n">
-        <v>7641129.11</v>
+        <v>798777.11</v>
+      </c>
+      <c r="D30" t="n">
+        <v>938402</v>
+      </c>
+      <c r="E30" t="n">
+        <v>629587</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2087150</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2003710</v>
+      </c>
+      <c r="H30" t="n">
+        <v>803431</v>
+      </c>
+      <c r="I30" t="n">
+        <v>250862</v>
+      </c>
+      <c r="J30" t="n">
+        <v>129210</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -837,7 +2125,49 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
         <v>38600.28</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -850,7 +2180,49 @@
         <v>67</v>
       </c>
       <c r="C32" t="n">
-        <v>42547594.5</v>
+        <v>3541939.14</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5772430.32</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5190222.54</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1571786.05</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3675718.56</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1001231.2</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7352858.81</v>
+      </c>
+      <c r="J32" t="n">
+        <v>5760931.17</v>
+      </c>
+      <c r="K32" t="n">
+        <v>2820933.98</v>
+      </c>
+      <c r="L32" t="n">
+        <v>3168345.01</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1832536.59</v>
+      </c>
+      <c r="N32" t="n">
+        <v>858661.13</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -863,7 +2235,49 @@
         <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>65141.88</v>
+        <v>16080.45</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7677.23</v>
+      </c>
+      <c r="E33" t="n">
+        <v>41384.2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -878,6 +2292,48 @@
       <c r="C34" t="n">
         <v>1417.4</v>
       </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -891,6 +2347,48 @@
       <c r="C35" t="n">
         <v>0</v>
       </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -902,7 +2400,49 @@
         <v>28</v>
       </c>
       <c r="C36" t="n">
-        <v>12825763.36</v>
+        <v>437505</v>
+      </c>
+      <c r="D36" t="n">
+        <v>803261</v>
+      </c>
+      <c r="E36" t="n">
+        <v>374064.3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>763080.27</v>
+      </c>
+      <c r="G36" t="n">
+        <v>86779</v>
+      </c>
+      <c r="H36" t="n">
+        <v>9300</v>
+      </c>
+      <c r="I36" t="n">
+        <v>9788156.1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>419286.02</v>
+      </c>
+      <c r="K36" t="n">
+        <v>32813</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>341.99</v>
+      </c>
+      <c r="O36" t="n">
+        <v>98522.60000000001</v>
+      </c>
+      <c r="P36" t="n">
+        <v>6581.62</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>6072.46</v>
       </c>
     </row>
     <row r="37">
@@ -915,7 +2455,49 @@
         <v>6</v>
       </c>
       <c r="C37" t="n">
-        <v>650467.25</v>
+        <v>19572</v>
+      </c>
+      <c r="D37" t="n">
+        <v>30388</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>588270</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>3888.25</v>
+      </c>
+      <c r="K37" t="n">
+        <v>4725</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>3624</v>
       </c>
     </row>
     <row r="38">
@@ -928,7 +2510,49 @@
         <v>1</v>
       </c>
       <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>55100</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -941,6 +2565,48 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
         <v>514166.44</v>
       </c>
     </row>
@@ -954,7 +2620,49 @@
         <v>16</v>
       </c>
       <c r="C40" t="n">
-        <v>53758188.34</v>
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>2253795.46</v>
+      </c>
+      <c r="L40" t="n">
+        <v>4613064.88</v>
+      </c>
+      <c r="M40" t="n">
+        <v>5514478.74</v>
+      </c>
+      <c r="N40" t="n">
+        <v>7889553.59</v>
+      </c>
+      <c r="O40" t="n">
+        <v>17974141.09</v>
+      </c>
+      <c r="P40" t="n">
+        <v>15466892.24</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>46262.34</v>
       </c>
     </row>
     <row r="41">
@@ -969,6 +2677,48 @@
       <c r="C41" t="n">
         <v>0</v>
       </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -980,7 +2730,49 @@
         <v>22</v>
       </c>
       <c r="C42" t="n">
-        <v>33374734.17</v>
+        <v>4265542.51</v>
+      </c>
+      <c r="D42" t="n">
+        <v>7330917.56</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4703333.54</v>
+      </c>
+      <c r="F42" t="n">
+        <v>842702.99</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6524700.43</v>
+      </c>
+      <c r="H42" t="n">
+        <v>699999.5</v>
+      </c>
+      <c r="I42" t="n">
+        <v>8990063</v>
+      </c>
+      <c r="J42" t="n">
+        <v>17474.64</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -995,6 +2787,48 @@
       <c r="C43" t="n">
         <v>0</v>
       </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1008,6 +2842,48 @@
       <c r="C44" t="n">
         <v>0</v>
       </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1019,7 +2895,49 @@
         <v>1</v>
       </c>
       <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
         <v>240655</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1034,6 +2952,48 @@
       <c r="C46" t="n">
         <v>0</v>
       </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1045,7 +3005,49 @@
         <v>2</v>
       </c>
       <c r="C47" t="n">
-        <v>1216175.75</v>
+        <v>515063.75</v>
+      </c>
+      <c r="D47" t="n">
+        <v>701112</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1060,6 +3062,48 @@
       <c r="C48" t="n">
         <v>0</v>
       </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1071,7 +3115,49 @@
         <v>36</v>
       </c>
       <c r="C49" t="n">
-        <v>78487432.45</v>
+        <v>8784393.800000001</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3126445.62</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3471517.25</v>
+      </c>
+      <c r="F49" t="n">
+        <v>9404014.83</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4677978.87</v>
+      </c>
+      <c r="H49" t="n">
+        <v>5370997.4</v>
+      </c>
+      <c r="I49" t="n">
+        <v>4602848.15</v>
+      </c>
+      <c r="J49" t="n">
+        <v>9614763.43</v>
+      </c>
+      <c r="K49" t="n">
+        <v>11963220.6</v>
+      </c>
+      <c r="L49" t="n">
+        <v>15021819.98</v>
+      </c>
+      <c r="M49" t="n">
+        <v>1052012.08</v>
+      </c>
+      <c r="N49" t="n">
+        <v>128864.26</v>
+      </c>
+      <c r="O49" t="n">
+        <v>1225360.18</v>
+      </c>
+      <c r="P49" t="n">
+        <v>43196</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1086,6 +3172,48 @@
       <c r="C50" t="n">
         <v>0</v>
       </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1097,7 +3225,49 @@
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>1823625.13</v>
+        <v>170284.47</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1398302.37</v>
+      </c>
+      <c r="E51" t="n">
+        <v>255038.29</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1110,7 +3280,49 @@
         <v>6</v>
       </c>
       <c r="C52" t="n">
-        <v>89726.92999999999</v>
+        <v>8835</v>
+      </c>
+      <c r="D52" t="n">
+        <v>55722.3</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>18721.03</v>
+      </c>
+      <c r="H52" t="n">
+        <v>6448.6</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1123,7 +3335,49 @@
         <v>14</v>
       </c>
       <c r="C53" t="n">
-        <v>5243408.53</v>
+        <v>245759</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1107034.85</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2524683.68</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1365931</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1136,7 +3390,49 @@
         <v>8</v>
       </c>
       <c r="C54" t="n">
-        <v>4511160.52</v>
+        <v>4308702.86</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>119216.34</v>
+      </c>
+      <c r="F54" t="n">
+        <v>31516.32</v>
+      </c>
+      <c r="G54" t="n">
+        <v>13125</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>38600</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1151,6 +3447,48 @@
       <c r="C55" t="n">
         <v>0</v>
       </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -1162,7 +3500,49 @@
         <v>6</v>
       </c>
       <c r="C56" t="n">
-        <v>7224392.34</v>
+        <v>394151</v>
+      </c>
+      <c r="D56" t="n">
+        <v>798423.05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>5605290.29</v>
+      </c>
+      <c r="F56" t="n">
+        <v>426528</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1177,6 +3557,48 @@
       <c r="C57" t="n">
         <v>0</v>
       </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1190,6 +3612,48 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1203,6 +3667,48 @@
       <c r="C59" t="n">
         <v>0</v>
       </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -1214,7 +3720,49 @@
         <v>21</v>
       </c>
       <c r="C60" t="n">
-        <v>17276567.55</v>
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1075107.25</v>
+      </c>
+      <c r="E60" t="n">
+        <v>294028</v>
+      </c>
+      <c r="F60" t="n">
+        <v>4102199</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3306492</v>
+      </c>
+      <c r="H60" t="n">
+        <v>483866</v>
+      </c>
+      <c r="I60" t="n">
+        <v>294000</v>
+      </c>
+      <c r="J60" t="n">
+        <v>3398400</v>
+      </c>
+      <c r="K60" t="n">
+        <v>158000</v>
+      </c>
+      <c r="L60" t="n">
+        <v>1004231</v>
+      </c>
+      <c r="M60" t="n">
+        <v>1303599</v>
+      </c>
+      <c r="N60" t="n">
+        <v>371995.3</v>
+      </c>
+      <c r="O60" t="n">
+        <v>8990</v>
+      </c>
+      <c r="P60" t="n">
+        <v>1173160</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>302500</v>
       </c>
     </row>
     <row r="61">
@@ -1227,7 +3775,49 @@
         <v>2</v>
       </c>
       <c r="C61" t="n">
-        <v>309009.69</v>
+        <v>305259.69</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>3750</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1240,7 +3830,49 @@
         <v>8</v>
       </c>
       <c r="C62" t="n">
-        <v>55776518.4</v>
+        <v>3956907</v>
+      </c>
+      <c r="D62" t="n">
+        <v>7885769</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1560021</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="n">
+        <v>15983973</v>
+      </c>
+      <c r="N62" t="n">
+        <v>10063603</v>
+      </c>
+      <c r="O62" t="n">
+        <v>5539538</v>
+      </c>
+      <c r="P62" t="n">
+        <v>10786707.4</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1255,6 +3887,48 @@
       <c r="C63" t="n">
         <v>0</v>
       </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -1266,7 +3940,49 @@
         <v>52</v>
       </c>
       <c r="C64" t="n">
-        <v>58185439.92</v>
+        <v>1361533.95</v>
+      </c>
+      <c r="D64" t="n">
+        <v>599909.8</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1471709.62</v>
+      </c>
+      <c r="F64" t="n">
+        <v>3597340.55</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1570078.09</v>
+      </c>
+      <c r="H64" t="n">
+        <v>4587669.4</v>
+      </c>
+      <c r="I64" t="n">
+        <v>4627916.88</v>
+      </c>
+      <c r="J64" t="n">
+        <v>6153068.73</v>
+      </c>
+      <c r="K64" t="n">
+        <v>4168503.94</v>
+      </c>
+      <c r="L64" t="n">
+        <v>3376134.44</v>
+      </c>
+      <c r="M64" t="n">
+        <v>16242211.27</v>
+      </c>
+      <c r="N64" t="n">
+        <v>3572619.95</v>
+      </c>
+      <c r="O64" t="n">
+        <v>2742491.8</v>
+      </c>
+      <c r="P64" t="n">
+        <v>4114251.5</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1279,7 +3995,49 @@
         <v>3</v>
       </c>
       <c r="C65" t="n">
-        <v>8165960.16</v>
+        <v>893273.36</v>
+      </c>
+      <c r="D65" t="n">
+        <v>7158268.8</v>
+      </c>
+      <c r="E65" t="n">
+        <v>114418</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1292,7 +4050,49 @@
         <v>3</v>
       </c>
       <c r="C66" t="n">
-        <v>108452.7</v>
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>73908</v>
+      </c>
+      <c r="N66" t="n">
+        <v>11895</v>
+      </c>
+      <c r="O66" t="n">
+        <v>22649.7</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1305,7 +4105,49 @@
         <v>2</v>
       </c>
       <c r="C67" t="n">
-        <v>8200</v>
+        <v>7850</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>350</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1318,7 +4160,49 @@
         <v>19</v>
       </c>
       <c r="C68" t="n">
-        <v>12264562.82</v>
+        <v>1430743</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1025616</v>
+      </c>
+      <c r="E68" t="n">
+        <v>264561</v>
+      </c>
+      <c r="F68" t="n">
+        <v>48025.36</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1549636.54</v>
+      </c>
+      <c r="H68" t="n">
+        <v>600556.1</v>
+      </c>
+      <c r="I68" t="n">
+        <v>1286066.58</v>
+      </c>
+      <c r="J68" t="n">
+        <v>2760650.4</v>
+      </c>
+      <c r="K68" t="n">
+        <v>920042.84</v>
+      </c>
+      <c r="L68" t="n">
+        <v>197889.79</v>
+      </c>
+      <c r="M68" t="n">
+        <v>1832612.77</v>
+      </c>
+      <c r="N68" t="n">
+        <v>259531.77</v>
+      </c>
+      <c r="O68" t="n">
+        <v>60818.82</v>
+      </c>
+      <c r="P68" t="n">
+        <v>13073</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>14738.85</v>
       </c>
     </row>
     <row r="69">
@@ -1331,7 +4215,49 @@
         <v>1</v>
       </c>
       <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
         <v>45064.24</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1344,7 +4270,49 @@
         <v>2</v>
       </c>
       <c r="C70" t="n">
-        <v>347395.52</v>
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>335643.52</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" t="n">
+        <v>11752</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1357,7 +4325,49 @@
         <v>7</v>
       </c>
       <c r="C71" t="n">
-        <v>6975560.97</v>
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
+        <v>470115.79</v>
+      </c>
+      <c r="L71" t="n">
+        <v>2986144</v>
+      </c>
+      <c r="M71" t="n">
+        <v>569069.12</v>
+      </c>
+      <c r="N71" t="n">
+        <v>2887034.06</v>
+      </c>
+      <c r="O71" t="n">
+        <v>63198</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1370,7 +4380,49 @@
         <v>5</v>
       </c>
       <c r="C72" t="n">
-        <v>865034.62</v>
+        <v>4719.62</v>
+      </c>
+      <c r="D72" t="n">
+        <v>685</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" t="n">
+        <v>414770</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" t="n">
+        <v>195520</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>249340</v>
       </c>
     </row>
     <row r="73">
@@ -1385,6 +4437,48 @@
       <c r="C73" t="n">
         <v>0</v>
       </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -1396,7 +4490,49 @@
         <v>1</v>
       </c>
       <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
         <v>11686</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1409,7 +4545,49 @@
         <v>11</v>
       </c>
       <c r="C75" t="n">
-        <v>1424479.58</v>
+        <v>729496.5</v>
+      </c>
+      <c r="D75" t="n">
+        <v>220117</v>
+      </c>
+      <c r="E75" t="n">
+        <v>34624.5</v>
+      </c>
+      <c r="F75" t="n">
+        <v>343592.58</v>
+      </c>
+      <c r="G75" t="n">
+        <v>25918</v>
+      </c>
+      <c r="H75" t="n">
+        <v>50231</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" t="n">
+        <v>3500</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
+        <v>15500</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" t="n">
+        <v>1500</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1422,7 +4600,49 @@
         <v>2</v>
       </c>
       <c r="C76" t="n">
-        <v>357106</v>
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>178739</v>
+      </c>
+      <c r="F76" t="n">
+        <v>178367</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1435,7 +4655,49 @@
         <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>192024.89</v>
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>61199.89</v>
+      </c>
+      <c r="G77" t="n">
+        <v>66895</v>
+      </c>
+      <c r="H77" t="n">
+        <v>21515</v>
+      </c>
+      <c r="I77" t="n">
+        <v>19800</v>
+      </c>
+      <c r="J77" t="n">
+        <v>22615</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1450,6 +4712,48 @@
       <c r="C78" t="n">
         <v>0</v>
       </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -1461,7 +4765,49 @@
         <v>4</v>
       </c>
       <c r="C79" t="n">
-        <v>70737.34</v>
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>57448.94</v>
+      </c>
+      <c r="H79" t="n">
+        <v>8550</v>
+      </c>
+      <c r="I79" t="n">
+        <v>4738.4</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1474,7 +4820,49 @@
         <v>6</v>
       </c>
       <c r="C80" t="n">
-        <v>12619245.46</v>
+        <v>93523.33</v>
+      </c>
+      <c r="D80" t="n">
+        <v>9287112.57</v>
+      </c>
+      <c r="E80" t="n">
+        <v>3191706.07</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>6244.79</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
+        <v>13714.89</v>
+      </c>
+      <c r="O80" t="n">
+        <v>26943.81</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1489,6 +4877,48 @@
       <c r="C81" t="n">
         <v>0</v>
       </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -1500,7 +4930,49 @@
         <v>18</v>
       </c>
       <c r="C82" t="n">
-        <v>6525493.61</v>
+        <v>52243.41</v>
+      </c>
+      <c r="D82" t="n">
+        <v>45437.71</v>
+      </c>
+      <c r="E82" t="n">
+        <v>34324.52</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>172747.82</v>
+      </c>
+      <c r="H82" t="n">
+        <v>681456.11</v>
+      </c>
+      <c r="I82" t="n">
+        <v>20508.14</v>
+      </c>
+      <c r="J82" t="n">
+        <v>955852.33</v>
+      </c>
+      <c r="K82" t="n">
+        <v>508562.68</v>
+      </c>
+      <c r="L82" t="n">
+        <v>50478.92</v>
+      </c>
+      <c r="M82" t="n">
+        <v>1189414.25</v>
+      </c>
+      <c r="N82" t="n">
+        <v>176009.12</v>
+      </c>
+      <c r="O82" t="n">
+        <v>1539934.74</v>
+      </c>
+      <c r="P82" t="n">
+        <v>769945.86</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>328578</v>
       </c>
     </row>
     <row r="83">
@@ -1513,7 +4985,49 @@
         <v>141</v>
       </c>
       <c r="C83" t="n">
-        <v>208230619.67</v>
+        <v>6359758.13</v>
+      </c>
+      <c r="D83" t="n">
+        <v>34686261.24</v>
+      </c>
+      <c r="E83" t="n">
+        <v>14021971.62</v>
+      </c>
+      <c r="F83" t="n">
+        <v>22343929.82</v>
+      </c>
+      <c r="G83" t="n">
+        <v>21189167.55</v>
+      </c>
+      <c r="H83" t="n">
+        <v>11053625.98</v>
+      </c>
+      <c r="I83" t="n">
+        <v>18042411.73</v>
+      </c>
+      <c r="J83" t="n">
+        <v>6861020.78</v>
+      </c>
+      <c r="K83" t="n">
+        <v>12761069.94</v>
+      </c>
+      <c r="L83" t="n">
+        <v>8972876.99</v>
+      </c>
+      <c r="M83" t="n">
+        <v>14518735.89</v>
+      </c>
+      <c r="N83" t="n">
+        <v>7749917.37</v>
+      </c>
+      <c r="O83" t="n">
+        <v>16779685.4</v>
+      </c>
+      <c r="P83" t="n">
+        <v>12824628.21</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>65559.02</v>
       </c>
     </row>
     <row r="84">
@@ -1526,7 +5040,49 @@
         <v>29</v>
       </c>
       <c r="C84" t="n">
-        <v>5772160.6</v>
+        <v>280900.45</v>
+      </c>
+      <c r="D84" t="n">
+        <v>261878.75</v>
+      </c>
+      <c r="E84" t="n">
+        <v>338937.77</v>
+      </c>
+      <c r="F84" t="n">
+        <v>133156.87</v>
+      </c>
+      <c r="G84" t="n">
+        <v>208505.62</v>
+      </c>
+      <c r="H84" t="n">
+        <v>145304.08</v>
+      </c>
+      <c r="I84" t="n">
+        <v>235343.67</v>
+      </c>
+      <c r="J84" t="n">
+        <v>388301.5</v>
+      </c>
+      <c r="K84" t="n">
+        <v>901983.4</v>
+      </c>
+      <c r="L84" t="n">
+        <v>490625.31</v>
+      </c>
+      <c r="M84" t="n">
+        <v>35332.32</v>
+      </c>
+      <c r="N84" t="n">
+        <v>1569758.07</v>
+      </c>
+      <c r="O84" t="n">
+        <v>521957.89</v>
+      </c>
+      <c r="P84" t="n">
+        <v>260174.9</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed .py file to reflect manufacturing focus. Also filterd on manufacturer of goods.
</commit_message>
<xml_diff>
--- a/Michigan Dataset.xlsx
+++ b/Michigan Dataset.xlsx
@@ -597,28 +597,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -642,28 +642,28 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>1712.5</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>107058</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>12600</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>3750</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>13200</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -715,16 +715,16 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -760,16 +760,16 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>44633.14</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>62214.5</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>9960</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>98350</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
@@ -888,28 +888,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -933,28 +933,28 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>831586</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>512700.5</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>8483</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>12485</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>5538</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
@@ -988,16 +988,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1033,16 +1033,16 @@
         <v>4847056.34</v>
       </c>
       <c r="R6" t="n">
-        <v>18488102.65</v>
+        <v>17645008.65</v>
       </c>
       <c r="S6" t="n">
-        <v>20318945.55</v>
+        <v>20063646.55</v>
       </c>
       <c r="T6" t="n">
-        <v>12999344.8</v>
+        <v>11981890.6</v>
       </c>
       <c r="U6" t="n">
-        <v>933927.4399999999</v>
+        <v>843705.6899999999</v>
       </c>
       <c r="V6" t="n">
         <v>235747</v>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>832710</v>
       </c>
       <c r="X7" t="n">
-        <v>4969.44</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
@@ -1188,19 +1188,19 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -1233,19 +1233,19 @@
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>1637350.76</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>76410</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>36072.62</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>108585.4</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -1470,91 +1470,91 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>5781905</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>13802950</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>5229554</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>1276350</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>8373940</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>3445700</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="n">
-        <v>3655950</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>2668396.5</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>9163795</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>10455140</v>
+        <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>18308443.12</v>
+        <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>4320130</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="AD16" t="n">
-        <v>3600.99</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
@@ -2052,91 +2052,91 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>3807976.32</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>2555795</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>4304547.14</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>1623062.16</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>716559.03</v>
+        <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>260348.16</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>12897576.2</v>
+        <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>7612218.77</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>6083490.52</v>
+        <v>0</v>
       </c>
       <c r="Z17" t="n">
-        <v>7962949.39</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>12526074</v>
+        <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>19784788.75</v>
+        <v>0</v>
       </c>
       <c r="AC17" t="n">
-        <v>18564322</v>
+        <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>12580638.29</v>
+        <v>0</v>
       </c>
       <c r="AE17" t="n">
         <v>0</v>
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>79663</v>
+        <v>0</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
@@ -2246,10 +2246,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
         <v>2</v>
@@ -2291,10 +2291,10 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>204338</v>
+        <v>72034</v>
       </c>
       <c r="R19" t="n">
-        <v>88319.07000000001</v>
+        <v>47489.77</v>
       </c>
       <c r="S19" t="n">
         <v>56365.08</v>
@@ -2446,25 +2446,25 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
       </c>
       <c r="J21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>2</v>
@@ -2491,25 +2491,25 @@
         <v>99937.7</v>
       </c>
       <c r="S21" t="n">
-        <v>315886</v>
+        <v>312596</v>
       </c>
       <c r="T21" t="n">
         <v>262825.2</v>
       </c>
       <c r="U21" t="n">
-        <v>368687.37</v>
+        <v>345309.87</v>
       </c>
       <c r="V21" t="n">
         <v>170325.93</v>
       </c>
       <c r="W21" t="n">
-        <v>480044.3</v>
+        <v>460488.19</v>
       </c>
       <c r="X21" t="n">
         <v>610818.0699999999</v>
       </c>
       <c r="Y21" t="n">
-        <v>823717.7</v>
+        <v>813952.7</v>
       </c>
       <c r="Z21" t="n">
         <v>729368.48</v>
@@ -2537,23 +2537,23 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
         <v>3</v>
       </c>
-      <c r="D22" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" t="n">
+      <c r="G22" t="n">
         <v>3</v>
       </c>
-      <c r="F22" t="n">
-        <v>4</v>
-      </c>
-      <c r="G22" t="n">
-        <v>4</v>
-      </c>
       <c r="H22" t="n">
         <v>1</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
@@ -2582,22 +2582,22 @@
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>13970874</v>
+        <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>16642823.13</v>
+        <v>349410.13</v>
       </c>
       <c r="S22" t="n">
-        <v>13502641.38</v>
+        <v>98332.22</v>
       </c>
       <c r="T22" t="n">
-        <v>25241715.65</v>
+        <v>509671.65</v>
       </c>
       <c r="U22" t="n">
-        <v>23296210.9</v>
+        <v>293094</v>
       </c>
       <c r="V22" t="n">
-        <v>3146459.51</v>
+        <v>348534.8</v>
       </c>
       <c r="W22" t="n">
         <v>417984.25</v>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="Z22" t="n">
-        <v>1796.92</v>
+        <v>0</v>
       </c>
       <c r="AA22" t="n">
         <v>0</v>
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>1968654.84</v>
+        <v>1911132.84</v>
       </c>
       <c r="R23" t="n">
         <v>1081822.99</v>
@@ -2831,34 +2831,34 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -2876,34 +2876,34 @@
         <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>11422.5</v>
+        <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>10567.2</v>
+        <v>5308.2</v>
       </c>
       <c r="T25" t="n">
-        <v>178743.25</v>
+        <v>0</v>
       </c>
       <c r="U25" t="n">
         <v>17852.99</v>
       </c>
       <c r="V25" t="n">
-        <v>17342</v>
+        <v>0</v>
       </c>
       <c r="W25" t="n">
-        <v>14222.75</v>
+        <v>0</v>
       </c>
       <c r="X25" t="n">
-        <v>4377</v>
+        <v>0</v>
       </c>
       <c r="Y25" t="n">
         <v>0</v>
       </c>
       <c r="Z25" t="n">
-        <v>79229.25</v>
+        <v>0</v>
       </c>
       <c r="AA25" t="n">
-        <v>3576</v>
+        <v>0</v>
       </c>
       <c r="AB25" t="n">
         <v>0</v>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="AD25" t="n">
-        <v>12076.31</v>
+        <v>0</v>
       </c>
       <c r="AE25" t="n">
         <v>0</v>
@@ -2925,91 +2925,91 @@
         </is>
       </c>
       <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
         <v>2</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" t="n">
+      <c r="H26" t="n">
         <v>2</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>2</v>
       </c>
-      <c r="G26" t="n">
-        <v>3</v>
-      </c>
-      <c r="H26" t="n">
-        <v>3</v>
-      </c>
-      <c r="I26" t="n">
-        <v>3</v>
-      </c>
       <c r="J26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>60383.03</v>
+        <v>0</v>
       </c>
       <c r="R26" t="n">
         <v>0</v>
       </c>
       <c r="S26" t="n">
-        <v>210404.4</v>
+        <v>15294.4</v>
       </c>
       <c r="T26" t="n">
-        <v>2501650.53</v>
+        <v>74106.53</v>
       </c>
       <c r="U26" t="n">
-        <v>1277774.52</v>
+        <v>107433.83</v>
       </c>
       <c r="V26" t="n">
-        <v>1577481</v>
+        <v>84918.42999999999</v>
       </c>
       <c r="W26" t="n">
-        <v>106823.91</v>
+        <v>97956.91</v>
       </c>
       <c r="X26" t="n">
-        <v>51330</v>
+        <v>8230</v>
       </c>
       <c r="Y26" t="n">
-        <v>273759.21</v>
+        <v>2097</v>
       </c>
       <c r="Z26" t="n">
-        <v>396323.83</v>
+        <v>1853.28</v>
       </c>
       <c r="AA26" t="n">
-        <v>502325.56</v>
+        <v>22268.56</v>
       </c>
       <c r="AB26" t="n">
-        <v>328751.52</v>
+        <v>0</v>
       </c>
       <c r="AC26" t="n">
-        <v>290738</v>
+        <v>0</v>
       </c>
       <c r="AD26" t="n">
-        <v>29625</v>
+        <v>0</v>
       </c>
       <c r="AE26" t="n">
         <v>0</v>
@@ -3031,10 +3031,10 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -3046,10 +3046,10 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -3076,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>20700</v>
+        <v>0</v>
       </c>
       <c r="U27" t="n">
-        <v>446000</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
         <v>0</v>
@@ -3091,10 +3091,10 @@
         <v>0</v>
       </c>
       <c r="Y27" t="n">
-        <v>13498.92</v>
+        <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>65185.64</v>
+        <v>0</v>
       </c>
       <c r="AA27" t="n">
         <v>0</v>
@@ -3119,40 +3119,40 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -3164,40 +3164,40 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>197393.91</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
-        <v>27451.75</v>
+        <v>0</v>
       </c>
       <c r="S28" t="n">
-        <v>24419.28</v>
+        <v>11942.26</v>
       </c>
       <c r="T28" t="n">
-        <v>754083.98</v>
+        <v>17083.98</v>
       </c>
       <c r="U28" t="n">
         <v>98936.50999999999</v>
       </c>
       <c r="V28" t="n">
-        <v>992103.87</v>
+        <v>0</v>
       </c>
       <c r="W28" t="n">
         <v>0</v>
       </c>
       <c r="X28" t="n">
-        <v>218177.18</v>
+        <v>0</v>
       </c>
       <c r="Y28" t="n">
-        <v>33420</v>
+        <v>0</v>
       </c>
       <c r="Z28" t="n">
-        <v>991520.84</v>
+        <v>0</v>
       </c>
       <c r="AA28" t="n">
         <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>889455.9</v>
+        <v>5250.5</v>
       </c>
       <c r="AC28" t="n">
         <v>0</v>
@@ -3222,16 +3222,16 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3267,16 +3267,16 @@
         <v>0</v>
       </c>
       <c r="S29" t="n">
-        <v>57984</v>
+        <v>9864</v>
       </c>
       <c r="T29" t="n">
-        <v>52748.89</v>
+        <v>28936.89</v>
       </c>
       <c r="U29" t="n">
-        <v>98837.96000000001</v>
+        <v>31562.96</v>
       </c>
       <c r="V29" t="n">
-        <v>19184</v>
+        <v>9404</v>
       </c>
       <c r="W29" t="n">
         <v>0</v>
@@ -3507,40 +3507,40 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N32" t="n">
         <v>0</v>
@@ -3552,40 +3552,40 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>3541939.14</v>
+        <v>7441</v>
       </c>
       <c r="R32" t="n">
-        <v>5772430.32</v>
+        <v>14300</v>
       </c>
       <c r="S32" t="n">
-        <v>5190222.54</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>1571786.05</v>
+        <v>102597.99</v>
       </c>
       <c r="U32" t="n">
-        <v>3675718.56</v>
+        <v>619327.98</v>
       </c>
       <c r="V32" t="n">
-        <v>1001231.2</v>
+        <v>98161</v>
       </c>
       <c r="W32" t="n">
-        <v>7352858.81</v>
+        <v>498938.3</v>
       </c>
       <c r="X32" t="n">
-        <v>5760931.17</v>
+        <v>1543359.59</v>
       </c>
       <c r="Y32" t="n">
-        <v>2820933.98</v>
+        <v>379241.66</v>
       </c>
       <c r="Z32" t="n">
-        <v>3168345.01</v>
+        <v>0</v>
       </c>
       <c r="AA32" t="n">
-        <v>1832536.59</v>
+        <v>0</v>
       </c>
       <c r="AB32" t="n">
-        <v>858661.13</v>
+        <v>0</v>
       </c>
       <c r="AC32" t="n">
         <v>0</v>
@@ -3701,7 +3701,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>1417.4</v>
+        <v>0</v>
       </c>
       <c r="R34" t="n">
         <v>0</v>
@@ -3895,28 +3895,28 @@
         </is>
       </c>
       <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
         <v>2</v>
       </c>
-      <c r="C36" t="n">
-        <v>3</v>
-      </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>2</v>
@@ -3931,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="N36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O36" t="n">
         <v>1</v>
@@ -3940,28 +3940,28 @@
         <v>1</v>
       </c>
       <c r="Q36" t="n">
-        <v>437505</v>
+        <v>12618</v>
       </c>
       <c r="R36" t="n">
-        <v>803261</v>
+        <v>802096</v>
       </c>
       <c r="S36" t="n">
-        <v>374064.3</v>
+        <v>22020.3</v>
       </c>
       <c r="T36" t="n">
-        <v>763080.27</v>
+        <v>727330.27</v>
       </c>
       <c r="U36" t="n">
-        <v>86779</v>
+        <v>0</v>
       </c>
       <c r="V36" t="n">
         <v>9300</v>
       </c>
       <c r="W36" t="n">
-        <v>9788156.1</v>
+        <v>65066.4</v>
       </c>
       <c r="X36" t="n">
-        <v>419286.02</v>
+        <v>14437.5</v>
       </c>
       <c r="Y36" t="n">
         <v>32813</v>
@@ -3976,7 +3976,7 @@
         <v>341.99</v>
       </c>
       <c r="AC36" t="n">
-        <v>98522.60000000001</v>
+        <v>69322.60000000001</v>
       </c>
       <c r="AD36" t="n">
         <v>6581.62</v>
@@ -4013,10 +4013,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
@@ -4034,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
         <v>19572</v>
@@ -4058,10 +4058,10 @@
         <v>0</v>
       </c>
       <c r="X37" t="n">
-        <v>3888.25</v>
+        <v>0</v>
       </c>
       <c r="Y37" t="n">
-        <v>4725</v>
+        <v>0</v>
       </c>
       <c r="Z37" t="n">
         <v>0</v>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
       <c r="AE37" t="n">
-        <v>3624</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="n">
         <v>0</v>
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="Y38" t="n">
-        <v>55100</v>
+        <v>0</v>
       </c>
       <c r="Z38" t="n">
         <v>0</v>
@@ -4228,7 +4228,7 @@
         <v>0</v>
       </c>
       <c r="P39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q39" t="n">
         <v>0</v>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="AE39" t="n">
-        <v>514166.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -4307,25 +4307,25 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="n">
         <v>0</v>
@@ -4352,25 +4352,25 @@
         <v>0</v>
       </c>
       <c r="Y40" t="n">
-        <v>2253795.46</v>
+        <v>0</v>
       </c>
       <c r="Z40" t="n">
-        <v>4613064.88</v>
+        <v>0</v>
       </c>
       <c r="AA40" t="n">
-        <v>5514478.74</v>
+        <v>0</v>
       </c>
       <c r="AB40" t="n">
-        <v>7889553.59</v>
+        <v>0</v>
       </c>
       <c r="AC40" t="n">
-        <v>17974141.09</v>
+        <v>0</v>
       </c>
       <c r="AD40" t="n">
-        <v>15466892.24</v>
+        <v>0</v>
       </c>
       <c r="AE40" t="n">
-        <v>46262.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -4477,28 +4477,28 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
@@ -4522,28 +4522,28 @@
         <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>4265542.51</v>
+        <v>22078</v>
       </c>
       <c r="R42" t="n">
-        <v>7330917.56</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>4703333.54</v>
+        <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>842702.99</v>
+        <v>89040</v>
       </c>
       <c r="U42" t="n">
-        <v>6524700.43</v>
+        <v>0</v>
       </c>
       <c r="V42" t="n">
-        <v>699999.5</v>
+        <v>0</v>
       </c>
       <c r="W42" t="n">
-        <v>8990063</v>
+        <v>0</v>
       </c>
       <c r="X42" t="n">
-        <v>17474.64</v>
+        <v>0</v>
       </c>
       <c r="Y42" t="n">
         <v>0</v>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -4816,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>240655</v>
+        <v>0</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
@@ -5156,34 +5156,34 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L49" t="n">
         <v>1</v>
@@ -5192,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="N49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O49" t="n">
         <v>1</v>
@@ -5201,34 +5201,34 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>8784393.800000001</v>
+        <v>561703.8</v>
       </c>
       <c r="R49" t="n">
-        <v>3126445.62</v>
+        <v>1441851.62</v>
       </c>
       <c r="S49" t="n">
-        <v>3471517.25</v>
+        <v>37805</v>
       </c>
       <c r="T49" t="n">
-        <v>9404014.83</v>
+        <v>110951.25</v>
       </c>
       <c r="U49" t="n">
-        <v>4677978.87</v>
+        <v>248858.06</v>
       </c>
       <c r="V49" t="n">
-        <v>5370997.4</v>
+        <v>241154.4</v>
       </c>
       <c r="W49" t="n">
-        <v>4602848.15</v>
+        <v>222107.15</v>
       </c>
       <c r="X49" t="n">
-        <v>9614763.43</v>
+        <v>246640.5</v>
       </c>
       <c r="Y49" t="n">
-        <v>11963220.6</v>
+        <v>308843.25</v>
       </c>
       <c r="Z49" t="n">
-        <v>15021819.98</v>
+        <v>861713.04</v>
       </c>
       <c r="AA49" t="n">
         <v>1052012.08</v>
@@ -5237,7 +5237,7 @@
         <v>128864.26</v>
       </c>
       <c r="AC49" t="n">
-        <v>1225360.18</v>
+        <v>94922.3</v>
       </c>
       <c r="AD49" t="n">
         <v>43196</v>
@@ -5350,13 +5350,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -5395,13 +5395,13 @@
         <v>0</v>
       </c>
       <c r="Q51" t="n">
-        <v>170284.47</v>
+        <v>8355</v>
       </c>
       <c r="R51" t="n">
-        <v>1398302.37</v>
+        <v>0</v>
       </c>
       <c r="S51" t="n">
-        <v>255038.29</v>
+        <v>0</v>
       </c>
       <c r="T51" t="n">
         <v>0</v>
@@ -5447,10 +5447,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -5459,7 +5459,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G52" t="n">
         <v>1</v>
@@ -5492,10 +5492,10 @@
         <v>0</v>
       </c>
       <c r="Q52" t="n">
-        <v>8835</v>
+        <v>0</v>
       </c>
       <c r="R52" t="n">
-        <v>55722.3</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
         <v>0</v>
@@ -5504,7 +5504,7 @@
         <v>0</v>
       </c>
       <c r="U52" t="n">
-        <v>18721.03</v>
+        <v>6667.3</v>
       </c>
       <c r="V52" t="n">
         <v>6448.6</v>
@@ -5544,16 +5544,16 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -5589,16 +5589,16 @@
         <v>0</v>
       </c>
       <c r="Q53" t="n">
-        <v>245759</v>
+        <v>0</v>
       </c>
       <c r="R53" t="n">
-        <v>1107034.85</v>
+        <v>0</v>
       </c>
       <c r="S53" t="n">
-        <v>2524683.68</v>
+        <v>0</v>
       </c>
       <c r="T53" t="n">
-        <v>1365931</v>
+        <v>0</v>
       </c>
       <c r="U53" t="n">
         <v>0</v>
@@ -5641,25 +5641,25 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -5686,25 +5686,25 @@
         <v>0</v>
       </c>
       <c r="Q54" t="n">
-        <v>4308702.86</v>
+        <v>65446.86</v>
       </c>
       <c r="R54" t="n">
         <v>0</v>
       </c>
       <c r="S54" t="n">
-        <v>119216.34</v>
+        <v>11016.84</v>
       </c>
       <c r="T54" t="n">
-        <v>31516.32</v>
+        <v>29541.32</v>
       </c>
       <c r="U54" t="n">
-        <v>13125</v>
+        <v>0</v>
       </c>
       <c r="V54" t="n">
         <v>0</v>
       </c>
       <c r="W54" t="n">
-        <v>38600</v>
+        <v>0</v>
       </c>
       <c r="X54" t="n">
         <v>0</v>
@@ -5838,10 +5838,10 @@
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
         <v>1</v>
@@ -5883,10 +5883,10 @@
         <v>394151</v>
       </c>
       <c r="R56" t="n">
-        <v>798423.05</v>
+        <v>146641</v>
       </c>
       <c r="S56" t="n">
-        <v>5605290.29</v>
+        <v>14896.8</v>
       </c>
       <c r="T56" t="n">
         <v>426528</v>
@@ -6226,91 +6226,91 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M60" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60" t="n">
         <v>0</v>
       </c>
       <c r="R60" t="n">
-        <v>1075107.25</v>
+        <v>0</v>
       </c>
       <c r="S60" t="n">
-        <v>294028</v>
+        <v>0</v>
       </c>
       <c r="T60" t="n">
-        <v>4102199</v>
+        <v>5409</v>
       </c>
       <c r="U60" t="n">
-        <v>3306492</v>
+        <v>0</v>
       </c>
       <c r="V60" t="n">
-        <v>483866</v>
+        <v>0</v>
       </c>
       <c r="W60" t="n">
-        <v>294000</v>
+        <v>0</v>
       </c>
       <c r="X60" t="n">
-        <v>3398400</v>
+        <v>0</v>
       </c>
       <c r="Y60" t="n">
-        <v>158000</v>
+        <v>0</v>
       </c>
       <c r="Z60" t="n">
-        <v>1004231</v>
+        <v>0</v>
       </c>
       <c r="AA60" t="n">
-        <v>1303599</v>
+        <v>0</v>
       </c>
       <c r="AB60" t="n">
-        <v>371995.3</v>
+        <v>0</v>
       </c>
       <c r="AC60" t="n">
-        <v>8990</v>
+        <v>0</v>
       </c>
       <c r="AD60" t="n">
-        <v>1173160</v>
+        <v>0</v>
       </c>
       <c r="AE60" t="n">
-        <v>302500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -6320,7 +6320,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -6365,7 +6365,7 @@
         <v>0</v>
       </c>
       <c r="Q61" t="n">
-        <v>305259.69</v>
+        <v>0</v>
       </c>
       <c r="R61" t="n">
         <v>0</v>
@@ -6417,13 +6417,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -6447,28 +6447,28 @@
         <v>0</v>
       </c>
       <c r="L62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P62" t="n">
         <v>0</v>
       </c>
       <c r="Q62" t="n">
-        <v>3956907</v>
+        <v>0</v>
       </c>
       <c r="R62" t="n">
-        <v>7885769</v>
+        <v>0</v>
       </c>
       <c r="S62" t="n">
-        <v>1560021</v>
+        <v>0</v>
       </c>
       <c r="T62" t="n">
         <v>0</v>
@@ -6492,16 +6492,16 @@
         <v>0</v>
       </c>
       <c r="AA62" t="n">
-        <v>15983973</v>
+        <v>0</v>
       </c>
       <c r="AB62" t="n">
-        <v>10063603</v>
+        <v>0</v>
       </c>
       <c r="AC62" t="n">
-        <v>5539538</v>
+        <v>0</v>
       </c>
       <c r="AD62" t="n">
-        <v>10786707.4</v>
+        <v>0</v>
       </c>
       <c r="AE62" t="n">
         <v>0</v>
@@ -6611,91 +6611,91 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M64" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P64" t="n">
         <v>0</v>
       </c>
       <c r="Q64" t="n">
-        <v>1361533.95</v>
+        <v>1092070.25</v>
       </c>
       <c r="R64" t="n">
-        <v>599909.8</v>
+        <v>587568.8</v>
       </c>
       <c r="S64" t="n">
-        <v>1471709.62</v>
+        <v>931828.22</v>
       </c>
       <c r="T64" t="n">
-        <v>3597340.55</v>
+        <v>1263488.05</v>
       </c>
       <c r="U64" t="n">
-        <v>1570078.09</v>
+        <v>1514391.69</v>
       </c>
       <c r="V64" t="n">
-        <v>4587669.4</v>
+        <v>2718097.9</v>
       </c>
       <c r="W64" t="n">
-        <v>4627916.88</v>
+        <v>2014407.75</v>
       </c>
       <c r="X64" t="n">
-        <v>6153068.73</v>
+        <v>1539278.94</v>
       </c>
       <c r="Y64" t="n">
-        <v>4168503.94</v>
+        <v>0</v>
       </c>
       <c r="Z64" t="n">
-        <v>3376134.44</v>
+        <v>0</v>
       </c>
       <c r="AA64" t="n">
-        <v>16242211.27</v>
+        <v>0</v>
       </c>
       <c r="AB64" t="n">
-        <v>3572619.95</v>
+        <v>0</v>
       </c>
       <c r="AC64" t="n">
-        <v>2742491.8</v>
+        <v>0</v>
       </c>
       <c r="AD64" t="n">
-        <v>4114251.5</v>
+        <v>0</v>
       </c>
       <c r="AE64" t="n">
         <v>0</v>
@@ -6708,13 +6708,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -6753,13 +6753,13 @@
         <v>0</v>
       </c>
       <c r="Q65" t="n">
-        <v>893273.36</v>
+        <v>0</v>
       </c>
       <c r="R65" t="n">
-        <v>7158268.8</v>
+        <v>0</v>
       </c>
       <c r="S65" t="n">
-        <v>114418</v>
+        <v>0</v>
       </c>
       <c r="T65" t="n">
         <v>0</v>
@@ -6835,13 +6835,13 @@
         <v>0</v>
       </c>
       <c r="L66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O66" t="n">
         <v>0</v>
@@ -6880,13 +6880,13 @@
         <v>0</v>
       </c>
       <c r="AA66" t="n">
-        <v>73908</v>
+        <v>0</v>
       </c>
       <c r="AB66" t="n">
-        <v>11895</v>
+        <v>0</v>
       </c>
       <c r="AC66" t="n">
-        <v>22649.7</v>
+        <v>0</v>
       </c>
       <c r="AD66" t="n">
         <v>0</v>
@@ -6902,13 +6902,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -6947,13 +6947,13 @@
         <v>0</v>
       </c>
       <c r="Q67" t="n">
-        <v>7850</v>
+        <v>0</v>
       </c>
       <c r="R67" t="n">
         <v>0</v>
       </c>
       <c r="S67" t="n">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="T67" t="n">
         <v>0</v>
@@ -7035,7 +7035,7 @@
         <v>2</v>
       </c>
       <c r="N68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O68" t="n">
         <v>1</v>
@@ -7080,7 +7080,7 @@
         <v>259531.77</v>
       </c>
       <c r="AC68" t="n">
-        <v>60818.82</v>
+        <v>844.8200000000001</v>
       </c>
       <c r="AD68" t="n">
         <v>13073</v>
@@ -7199,7 +7199,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -7244,7 +7244,7 @@
         <v>0</v>
       </c>
       <c r="S70" t="n">
-        <v>335643.52</v>
+        <v>0</v>
       </c>
       <c r="T70" t="n">
         <v>0</v>
@@ -7314,19 +7314,19 @@
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O71" t="n">
         <v>0</v>
@@ -7359,19 +7359,19 @@
         <v>0</v>
       </c>
       <c r="Y71" t="n">
-        <v>470115.79</v>
+        <v>0</v>
       </c>
       <c r="Z71" t="n">
-        <v>2986144</v>
+        <v>0</v>
       </c>
       <c r="AA71" t="n">
-        <v>569069.12</v>
+        <v>0</v>
       </c>
       <c r="AB71" t="n">
-        <v>2887034.06</v>
+        <v>0</v>
       </c>
       <c r="AC71" t="n">
-        <v>63198</v>
+        <v>0</v>
       </c>
       <c r="AD71" t="n">
         <v>0</v>
@@ -7693,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7705,13 +7705,13 @@
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75" t="n">
         <v>0</v>
       </c>
       <c r="M75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N75" t="n">
         <v>0</v>
@@ -7738,7 +7738,7 @@
         <v>25918</v>
       </c>
       <c r="V75" t="n">
-        <v>50231</v>
+        <v>0</v>
       </c>
       <c r="W75" t="n">
         <v>0</v>
@@ -7750,13 +7750,13 @@
         <v>0</v>
       </c>
       <c r="Z75" t="n">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="AA75" t="n">
         <v>0</v>
       </c>
       <c r="AB75" t="n">
-        <v>15500</v>
+        <v>0</v>
       </c>
       <c r="AC75" t="n">
         <v>0</v>
@@ -7781,10 +7781,10 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -7826,10 +7826,10 @@
         <v>0</v>
       </c>
       <c r="S76" t="n">
-        <v>178739</v>
+        <v>0</v>
       </c>
       <c r="T76" t="n">
-        <v>178367</v>
+        <v>0</v>
       </c>
       <c r="U76" t="n">
         <v>0</v>
@@ -8078,13 +8078,13 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -8123,13 +8123,13 @@
         <v>0</v>
       </c>
       <c r="U79" t="n">
-        <v>57448.94</v>
+        <v>0</v>
       </c>
       <c r="V79" t="n">
-        <v>8550</v>
+        <v>0</v>
       </c>
       <c r="W79" t="n">
-        <v>4738.4</v>
+        <v>0</v>
       </c>
       <c r="X79" t="n">
         <v>0</v>
@@ -8163,13 +8163,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -8184,7 +8184,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -8196,10 +8196,10 @@
         <v>0</v>
       </c>
       <c r="M80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O80" t="n">
         <v>0</v>
@@ -8208,13 +8208,13 @@
         <v>0</v>
       </c>
       <c r="Q80" t="n">
-        <v>93523.33</v>
+        <v>0</v>
       </c>
       <c r="R80" t="n">
-        <v>9287112.57</v>
+        <v>0</v>
       </c>
       <c r="S80" t="n">
-        <v>3191706.07</v>
+        <v>0</v>
       </c>
       <c r="T80" t="n">
         <v>0</v>
@@ -8229,7 +8229,7 @@
         <v>0</v>
       </c>
       <c r="X80" t="n">
-        <v>6244.79</v>
+        <v>0</v>
       </c>
       <c r="Y80" t="n">
         <v>0</v>
@@ -8241,10 +8241,10 @@
         <v>0</v>
       </c>
       <c r="AB80" t="n">
-        <v>13714.89</v>
+        <v>0</v>
       </c>
       <c r="AC80" t="n">
-        <v>26943.81</v>
+        <v>0</v>
       </c>
       <c r="AD80" t="n">
         <v>0</v>
@@ -8357,94 +8357,94 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q82" t="n">
-        <v>52243.41</v>
+        <v>0</v>
       </c>
       <c r="R82" t="n">
-        <v>45437.71</v>
+        <v>0</v>
       </c>
       <c r="S82" t="n">
-        <v>34324.52</v>
+        <v>0</v>
       </c>
       <c r="T82" t="n">
         <v>0</v>
       </c>
       <c r="U82" t="n">
-        <v>172747.82</v>
+        <v>0</v>
       </c>
       <c r="V82" t="n">
-        <v>681456.11</v>
+        <v>0</v>
       </c>
       <c r="W82" t="n">
-        <v>20508.14</v>
+        <v>0</v>
       </c>
       <c r="X82" t="n">
-        <v>955852.33</v>
+        <v>0</v>
       </c>
       <c r="Y82" t="n">
-        <v>508562.68</v>
+        <v>0</v>
       </c>
       <c r="Z82" t="n">
-        <v>50478.92</v>
+        <v>0</v>
       </c>
       <c r="AA82" t="n">
-        <v>1189414.25</v>
+        <v>0</v>
       </c>
       <c r="AB82" t="n">
-        <v>176009.12</v>
+        <v>0</v>
       </c>
       <c r="AC82" t="n">
-        <v>1539934.74</v>
+        <v>0</v>
       </c>
       <c r="AD82" t="n">
-        <v>769945.86</v>
+        <v>0</v>
       </c>
       <c r="AE82" t="n">
-        <v>328578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -8454,94 +8454,94 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C83" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E83" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G83" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H83" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I83" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K83" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M83" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N83" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="O83" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q83" t="n">
-        <v>6359758.13</v>
+        <v>282922.26</v>
       </c>
       <c r="R83" t="n">
-        <v>34686261.24</v>
+        <v>333172.58</v>
       </c>
       <c r="S83" t="n">
-        <v>14021971.62</v>
+        <v>790163.34</v>
       </c>
       <c r="T83" t="n">
-        <v>22343929.82</v>
+        <v>845832.22</v>
       </c>
       <c r="U83" t="n">
-        <v>21189167.55</v>
+        <v>328762.62</v>
       </c>
       <c r="V83" t="n">
-        <v>11053625.98</v>
+        <v>82276.74000000001</v>
       </c>
       <c r="W83" t="n">
-        <v>18042411.73</v>
+        <v>46920.16</v>
       </c>
       <c r="X83" t="n">
-        <v>6861020.78</v>
+        <v>0</v>
       </c>
       <c r="Y83" t="n">
-        <v>12761069.94</v>
+        <v>0</v>
       </c>
       <c r="Z83" t="n">
-        <v>8972876.99</v>
+        <v>0</v>
       </c>
       <c r="AA83" t="n">
-        <v>14518735.89</v>
+        <v>28117.41</v>
       </c>
       <c r="AB83" t="n">
-        <v>7749917.37</v>
+        <v>0</v>
       </c>
       <c r="AC83" t="n">
-        <v>16779685.4</v>
+        <v>10126.1</v>
       </c>
       <c r="AD83" t="n">
-        <v>12824628.21</v>
+        <v>6475.2</v>
       </c>
       <c r="AE83" t="n">
-        <v>65559.02</v>
+        <v>7402.02</v>
       </c>
     </row>
     <row r="84">
@@ -8551,10 +8551,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="n">
         <v>2</v>
@@ -8578,13 +8578,13 @@
         <v>2</v>
       </c>
       <c r="K84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N84" t="n">
         <v>1</v>
@@ -8596,10 +8596,10 @@
         <v>0</v>
       </c>
       <c r="Q84" t="n">
-        <v>280900.45</v>
+        <v>238987</v>
       </c>
       <c r="R84" t="n">
-        <v>261878.75</v>
+        <v>251978.75</v>
       </c>
       <c r="S84" t="n">
         <v>338937.77</v>
@@ -8623,13 +8623,13 @@
         <v>901983.4</v>
       </c>
       <c r="Z84" t="n">
-        <v>490625.31</v>
+        <v>481160.31</v>
       </c>
       <c r="AA84" t="n">
-        <v>35332.32</v>
+        <v>17407.32</v>
       </c>
       <c r="AB84" t="n">
-        <v>1569758.07</v>
+        <v>1555453.07</v>
       </c>
       <c r="AC84" t="n">
         <v>521957.89</v>

</xml_diff>

<commit_message>
Added employee data from 2008-2017 for manufacturing companies
</commit_message>
<xml_diff>
--- a/Michigan Dataset.xlsx
+++ b/Michigan Dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE84"/>
+  <dimension ref="A1:AO84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,56 @@
           <t>Federal Contract Compensation - 2022</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2008</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2009</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2010</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2011</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2012</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2013</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2014</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2015</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2016</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturing Employees on Avg. - 2017</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -686,6 +736,36 @@
       <c r="AE2" t="n">
         <v>0</v>
       </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -783,6 +863,36 @@
       <c r="AE3" t="n">
         <v>0</v>
       </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -880,6 +990,36 @@
       <c r="AE4" t="n">
         <v>0</v>
       </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -977,6 +1117,36 @@
       <c r="AE5" t="n">
         <v>0</v>
       </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1074,6 +1244,36 @@
       <c r="AE6" t="n">
         <v>0</v>
       </c>
+      <c r="AF6" t="n">
+        <v>238</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>180</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>257</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>462</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>95</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>125</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>125</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>105</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1171,6 +1371,36 @@
       <c r="AE7" t="n">
         <v>0</v>
       </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>12</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>27</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>27</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1268,6 +1498,36 @@
       <c r="AE8" t="n">
         <v>1489.44</v>
       </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1365,6 +1625,36 @@
       <c r="AE9" t="n">
         <v>0</v>
       </c>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1462,6 +1752,36 @@
       <c r="AE10" t="n">
         <v>0</v>
       </c>
+      <c r="AF10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1559,6 +1879,36 @@
       <c r="AE11" t="n">
         <v>0</v>
       </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1656,6 +2006,36 @@
       <c r="AE12" t="n">
         <v>0</v>
       </c>
+      <c r="AF12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1753,6 +2133,36 @@
       <c r="AE13" t="n">
         <v>0</v>
       </c>
+      <c r="AF13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1850,6 +2260,36 @@
       <c r="AE14" t="n">
         <v>0</v>
       </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1947,6 +2387,36 @@
       <c r="AE15" t="n">
         <v>0</v>
       </c>
+      <c r="AF15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -2044,6 +2514,36 @@
       <c r="AE16" t="n">
         <v>0</v>
       </c>
+      <c r="AF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -2141,6 +2641,36 @@
       <c r="AE17" t="n">
         <v>0</v>
       </c>
+      <c r="AF17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -2238,6 +2768,36 @@
       <c r="AE18" t="n">
         <v>0</v>
       </c>
+      <c r="AF18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -2335,6 +2895,36 @@
       <c r="AE19" t="n">
         <v>0</v>
       </c>
+      <c r="AF19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>390</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -2432,6 +3022,36 @@
       <c r="AE20" t="n">
         <v>0</v>
       </c>
+      <c r="AF20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2529,6 +3149,36 @@
       <c r="AE21" t="n">
         <v>131595.54</v>
       </c>
+      <c r="AF21" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>20</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>40</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -2626,6 +3276,36 @@
       <c r="AE22" t="n">
         <v>0</v>
       </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>79</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>87</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>38</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2723,6 +3403,36 @@
       <c r="AE23" t="n">
         <v>0</v>
       </c>
+      <c r="AF23" t="n">
+        <v>600</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>650</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>650</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>497</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>507</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>500</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>500</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -2820,6 +3530,36 @@
       <c r="AE24" t="n">
         <v>0</v>
       </c>
+      <c r="AF24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -2917,6 +3657,36 @@
       <c r="AE25" t="n">
         <v>0</v>
       </c>
+      <c r="AF25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -3014,6 +3784,36 @@
       <c r="AE26" t="n">
         <v>0</v>
       </c>
+      <c r="AF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>112</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>112</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>220</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>110</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -3111,6 +3911,36 @@
       <c r="AE27" t="n">
         <v>0</v>
       </c>
+      <c r="AF27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -3208,6 +4038,36 @@
       <c r="AE28" t="n">
         <v>0</v>
       </c>
+      <c r="AF28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>147</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>147</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>147</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -3305,6 +4165,36 @@
       <c r="AE29" t="n">
         <v>0</v>
       </c>
+      <c r="AF29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>26</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>26</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>31</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -3402,6 +4292,36 @@
       <c r="AE30" t="n">
         <v>0</v>
       </c>
+      <c r="AF30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>70</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>65</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>130</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -3499,6 +4419,36 @@
       <c r="AE31" t="n">
         <v>0</v>
       </c>
+      <c r="AF31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>60</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -3596,6 +4546,36 @@
       <c r="AE32" t="n">
         <v>0</v>
       </c>
+      <c r="AF32" t="n">
+        <v>130</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>148</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>28</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>145</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>26</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>26</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>26</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -3693,6 +4673,36 @@
       <c r="AE33" t="n">
         <v>0</v>
       </c>
+      <c r="AF33" t="n">
+        <v>70</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>70</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -3790,6 +4800,36 @@
       <c r="AE34" t="n">
         <v>0</v>
       </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -3887,6 +4927,36 @@
       <c r="AE35" t="n">
         <v>0</v>
       </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -3984,6 +5054,36 @@
       <c r="AE36" t="n">
         <v>6072.46</v>
       </c>
+      <c r="AF36" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>163</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>163</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>163</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM36" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN36" t="n">
+        <v>17</v>
+      </c>
+      <c r="AO36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -4081,6 +5181,36 @@
       <c r="AE37" t="n">
         <v>0</v>
       </c>
+      <c r="AF37" t="n">
+        <v>650</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>650</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI37" t="n">
+        <v>650</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -4178,6 +5308,36 @@
       <c r="AE38" t="n">
         <v>0</v>
       </c>
+      <c r="AF38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -4275,6 +5435,36 @@
       <c r="AE39" t="n">
         <v>0</v>
       </c>
+      <c r="AF39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -4372,6 +5562,36 @@
       <c r="AE40" t="n">
         <v>0</v>
       </c>
+      <c r="AF40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -4469,6 +5689,36 @@
       <c r="AE41" t="n">
         <v>0</v>
       </c>
+      <c r="AF41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -4566,6 +5816,36 @@
       <c r="AE42" t="n">
         <v>0</v>
       </c>
+      <c r="AF42" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI42" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -4663,6 +5943,36 @@
       <c r="AE43" t="n">
         <v>0</v>
       </c>
+      <c r="AF43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -4760,6 +6070,36 @@
       <c r="AE44" t="n">
         <v>0</v>
       </c>
+      <c r="AF44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -4857,6 +6197,36 @@
       <c r="AE45" t="n">
         <v>0</v>
       </c>
+      <c r="AF45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -4954,6 +6324,36 @@
       <c r="AE46" t="n">
         <v>0</v>
       </c>
+      <c r="AF46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -5051,6 +6451,36 @@
       <c r="AE47" t="n">
         <v>0</v>
       </c>
+      <c r="AF47" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -5148,6 +6578,36 @@
       <c r="AE48" t="n">
         <v>0</v>
       </c>
+      <c r="AF48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -5245,6 +6705,36 @@
       <c r="AE49" t="n">
         <v>0</v>
       </c>
+      <c r="AF49" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG49" t="n">
+        <v>14</v>
+      </c>
+      <c r="AH49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AJ49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AL49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AM49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN49" t="n">
+        <v>18</v>
+      </c>
+      <c r="AO49" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -5342,6 +6832,36 @@
       <c r="AE50" t="n">
         <v>0</v>
       </c>
+      <c r="AF50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -5439,6 +6959,36 @@
       <c r="AE51" t="n">
         <v>0</v>
       </c>
+      <c r="AF51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -5536,6 +7086,36 @@
       <c r="AE52" t="n">
         <v>0</v>
       </c>
+      <c r="AF52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ52" t="n">
+        <v>130</v>
+      </c>
+      <c r="AK52" t="n">
+        <v>100</v>
+      </c>
+      <c r="AL52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -5633,6 +7213,36 @@
       <c r="AE53" t="n">
         <v>0</v>
       </c>
+      <c r="AF53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -5730,6 +7340,36 @@
       <c r="AE54" t="n">
         <v>0</v>
       </c>
+      <c r="AF54" t="n">
+        <v>222</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH54" t="n">
+        <v>222</v>
+      </c>
+      <c r="AI54" t="n">
+        <v>222</v>
+      </c>
+      <c r="AJ54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -5827,6 +7467,36 @@
       <c r="AE55" t="n">
         <v>0</v>
       </c>
+      <c r="AF55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -5924,6 +7594,36 @@
       <c r="AE56" t="n">
         <v>0</v>
       </c>
+      <c r="AF56" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH56" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI56" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -6021,6 +7721,36 @@
       <c r="AE57" t="n">
         <v>0</v>
       </c>
+      <c r="AF57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -6118,6 +7848,36 @@
       <c r="AE58" t="n">
         <v>0</v>
       </c>
+      <c r="AF58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -6215,6 +7975,36 @@
       <c r="AE59" t="n">
         <v>0</v>
       </c>
+      <c r="AF59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -6312,6 +8102,36 @@
       <c r="AE60" t="n">
         <v>0</v>
       </c>
+      <c r="AF60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI60" t="n">
+        <v>19</v>
+      </c>
+      <c r="AJ60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -6409,6 +8229,36 @@
       <c r="AE61" t="n">
         <v>0</v>
       </c>
+      <c r="AF61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM61" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -6506,6 +8356,36 @@
       <c r="AE62" t="n">
         <v>0</v>
       </c>
+      <c r="AF62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -6603,6 +8483,36 @@
       <c r="AE63" t="n">
         <v>0</v>
       </c>
+      <c r="AF63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -6700,6 +8610,36 @@
       <c r="AE64" t="n">
         <v>0</v>
       </c>
+      <c r="AF64" t="n">
+        <v>19</v>
+      </c>
+      <c r="AG64" t="n">
+        <v>19</v>
+      </c>
+      <c r="AH64" t="n">
+        <v>19</v>
+      </c>
+      <c r="AI64" t="n">
+        <v>19</v>
+      </c>
+      <c r="AJ64" t="n">
+        <v>19</v>
+      </c>
+      <c r="AK64" t="n">
+        <v>14</v>
+      </c>
+      <c r="AL64" t="n">
+        <v>14</v>
+      </c>
+      <c r="AM64" t="n">
+        <v>14</v>
+      </c>
+      <c r="AN64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -6797,6 +8737,36 @@
       <c r="AE65" t="n">
         <v>0</v>
       </c>
+      <c r="AF65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -6894,6 +8864,36 @@
       <c r="AE66" t="n">
         <v>0</v>
       </c>
+      <c r="AF66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -6991,6 +8991,36 @@
       <c r="AE67" t="n">
         <v>0</v>
       </c>
+      <c r="AF67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -7088,6 +9118,36 @@
       <c r="AE68" t="n">
         <v>14738.85</v>
       </c>
+      <c r="AF68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AG68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AH68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AI68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AJ68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AK68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AL68" t="n">
+        <v>75</v>
+      </c>
+      <c r="AM68" t="n">
+        <v>100</v>
+      </c>
+      <c r="AN68" t="n">
+        <v>50</v>
+      </c>
+      <c r="AO68" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -7185,6 +9245,36 @@
       <c r="AE69" t="n">
         <v>0</v>
       </c>
+      <c r="AF69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI69" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -7282,6 +9372,36 @@
       <c r="AE70" t="n">
         <v>0</v>
       </c>
+      <c r="AF70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -7379,6 +9499,36 @@
       <c r="AE71" t="n">
         <v>0</v>
       </c>
+      <c r="AF71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -7476,6 +9626,36 @@
       <c r="AE72" t="n">
         <v>249340</v>
       </c>
+      <c r="AF72" t="n">
+        <v>47</v>
+      </c>
+      <c r="AG72" t="n">
+        <v>47</v>
+      </c>
+      <c r="AH72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -7573,6 +9753,36 @@
       <c r="AE73" t="n">
         <v>0</v>
       </c>
+      <c r="AF73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -7670,6 +9880,36 @@
       <c r="AE74" t="n">
         <v>0</v>
       </c>
+      <c r="AF74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI74" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -7767,6 +10007,36 @@
       <c r="AE75" t="n">
         <v>0</v>
       </c>
+      <c r="AF75" t="n">
+        <v>53</v>
+      </c>
+      <c r="AG75" t="n">
+        <v>63</v>
+      </c>
+      <c r="AH75" t="n">
+        <v>65</v>
+      </c>
+      <c r="AI75" t="n">
+        <v>228</v>
+      </c>
+      <c r="AJ75" t="n">
+        <v>176</v>
+      </c>
+      <c r="AK75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -7864,6 +10134,36 @@
       <c r="AE76" t="n">
         <v>0</v>
       </c>
+      <c r="AF76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -7961,6 +10261,36 @@
       <c r="AE77" t="n">
         <v>0</v>
       </c>
+      <c r="AF77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI77" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ77" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK77" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL77" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM77" t="n">
+        <v>9</v>
+      </c>
+      <c r="AN77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -8058,6 +10388,36 @@
       <c r="AE78" t="n">
         <v>0</v>
       </c>
+      <c r="AF78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -8155,6 +10515,36 @@
       <c r="AE79" t="n">
         <v>0</v>
       </c>
+      <c r="AF79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -8252,6 +10642,36 @@
       <c r="AE80" t="n">
         <v>0</v>
       </c>
+      <c r="AF80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -8349,6 +10769,36 @@
       <c r="AE81" t="n">
         <v>0</v>
       </c>
+      <c r="AF81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -8446,6 +10896,36 @@
       <c r="AE82" t="n">
         <v>0</v>
       </c>
+      <c r="AF82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -8543,6 +11023,36 @@
       <c r="AE83" t="n">
         <v>7402.02</v>
       </c>
+      <c r="AF83" t="n">
+        <v>451</v>
+      </c>
+      <c r="AG83" t="n">
+        <v>564</v>
+      </c>
+      <c r="AH83" t="n">
+        <v>491</v>
+      </c>
+      <c r="AI83" t="n">
+        <v>548</v>
+      </c>
+      <c r="AJ83" t="n">
+        <v>258</v>
+      </c>
+      <c r="AK83" t="n">
+        <v>54</v>
+      </c>
+      <c r="AL83" t="n">
+        <v>54</v>
+      </c>
+      <c r="AM83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -8639,6 +11149,36 @@
       </c>
       <c r="AE84" t="n">
         <v>0</v>
+      </c>
+      <c r="AF84" t="n">
+        <v>85</v>
+      </c>
+      <c r="AG84" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH84" t="n">
+        <v>48</v>
+      </c>
+      <c r="AI84" t="n">
+        <v>90</v>
+      </c>
+      <c r="AJ84" t="n">
+        <v>54</v>
+      </c>
+      <c r="AK84" t="n">
+        <v>90</v>
+      </c>
+      <c r="AL84" t="n">
+        <v>90</v>
+      </c>
+      <c r="AM84" t="n">
+        <v>121</v>
+      </c>
+      <c r="AN84" t="n">
+        <v>102</v>
+      </c>
+      <c r="AO84" t="n">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Employees earned on average rather than cumulative over all manufacturing HUBZone Businesses
</commit_message>
<xml_diff>
--- a/Michigan Dataset.xlsx
+++ b/Michigan Dataset.xlsx
@@ -1245,19 +1245,19 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>238</v>
+        <v>59.5</v>
       </c>
       <c r="AG6" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="AH6" t="n">
-        <v>257</v>
+        <v>128.5</v>
       </c>
       <c r="AI6" t="n">
-        <v>462</v>
+        <v>231</v>
       </c>
       <c r="AJ6" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="AK6" t="n">
         <v>95</v>
@@ -2896,19 +2896,19 @@
         <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="AG19" t="n">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="AH19" t="n">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="AI19" t="n">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="AJ19" t="n">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="AK19" t="n">
         <v>0</v>
@@ -3171,13 +3171,13 @@
         <v>30</v>
       </c>
       <c r="AM21" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AN21" t="n">
         <v>20</v>
       </c>
       <c r="AO21" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -3289,10 +3289,10 @@
         <v>32</v>
       </c>
       <c r="AJ22" t="n">
-        <v>79</v>
+        <v>26.33333333333333</v>
       </c>
       <c r="AK22" t="n">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="AL22" t="n">
         <v>38</v>
@@ -3800,13 +3800,13 @@
         <v>1</v>
       </c>
       <c r="AK26" t="n">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="AL26" t="n">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="AM26" t="n">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="AN26" t="n">
         <v>110</v>
@@ -4314,7 +4314,7 @@
         <v>65</v>
       </c>
       <c r="AM30" t="n">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="AN30" t="n">
         <v>0</v>
@@ -4550,16 +4550,16 @@
         <v>130</v>
       </c>
       <c r="AG32" t="n">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="AH32" t="n">
         <v>0</v>
       </c>
       <c r="AI32" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="AJ32" t="n">
-        <v>145</v>
+        <v>72.5</v>
       </c>
       <c r="AK32" t="n">
         <v>22</v>
@@ -5058,13 +5058,13 @@
         <v>16</v>
       </c>
       <c r="AG36" t="n">
-        <v>163</v>
+        <v>81.5</v>
       </c>
       <c r="AH36" t="n">
-        <v>163</v>
+        <v>81.5</v>
       </c>
       <c r="AI36" t="n">
-        <v>163</v>
+        <v>81.5</v>
       </c>
       <c r="AJ36" t="n">
         <v>0</v>
@@ -5079,7 +5079,7 @@
         <v>18</v>
       </c>
       <c r="AN36" t="n">
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AO36" t="n">
         <v>0</v>
@@ -7099,7 +7099,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" t="n">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="AK52" t="n">
         <v>100</v>
@@ -9140,13 +9140,13 @@
         <v>75</v>
       </c>
       <c r="AM68" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="AN68" t="n">
         <v>50</v>
       </c>
       <c r="AO68" t="n">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69">
@@ -10014,10 +10014,10 @@
         <v>63</v>
       </c>
       <c r="AH75" t="n">
-        <v>65</v>
+        <v>32.5</v>
       </c>
       <c r="AI75" t="n">
-        <v>228</v>
+        <v>114</v>
       </c>
       <c r="AJ75" t="n">
         <v>176</v>
@@ -11024,19 +11024,19 @@
         <v>7402.02</v>
       </c>
       <c r="AF83" t="n">
-        <v>451</v>
+        <v>112.75</v>
       </c>
       <c r="AG83" t="n">
-        <v>564</v>
+        <v>141</v>
       </c>
       <c r="AH83" t="n">
-        <v>491</v>
+        <v>163.6666666666667</v>
       </c>
       <c r="AI83" t="n">
-        <v>548</v>
+        <v>137</v>
       </c>
       <c r="AJ83" t="n">
-        <v>258</v>
+        <v>86</v>
       </c>
       <c r="AK83" t="n">
         <v>54</v>
@@ -11151,34 +11151,34 @@
         <v>0</v>
       </c>
       <c r="AF84" t="n">
-        <v>85</v>
+        <v>42.5</v>
       </c>
       <c r="AG84" t="n">
         <v>28</v>
       </c>
       <c r="AH84" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="AI84" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AJ84" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="AK84" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AL84" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AM84" t="n">
-        <v>121</v>
+        <v>40.33333333333334</v>
       </c>
       <c r="AN84" t="n">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="AO84" t="n">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>